<commit_message>
26.05.2022 WriteExcel - TakeScreenShot
</commit_message>
<xml_diff>
--- a/src/Resources/ulkeler.xlsx
+++ b/src/Resources/ulkeler.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2CB33B-669E-47A2-95A0-4D1E55E9CD82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0D95E5-78A1-4606-9B45-E336EF132BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="578">
   <si>
     <t>Ülke (İngilizce)</t>
   </si>
@@ -1741,6 +1741,21 @@
   </si>
   <si>
     <t>Zimbabve</t>
+  </si>
+  <si>
+    <t>Nufus</t>
+  </si>
+  <si>
+    <t>1500000</t>
+  </si>
+  <si>
+    <t>250000</t>
+  </si>
+  <si>
+    <t>54000</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -2167,18 +2182,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D191"/>
+  <dimension ref="A1:E191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="4" width="25.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2191,8 +2206,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -2205,8 +2223,11 @@
       <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -2220,7 +2241,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -2234,7 +2255,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -2248,7 +2269,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -2262,7 +2283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -2276,7 +2297,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -2290,7 +2311,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -2304,7 +2325,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -2317,8 +2338,11 @@
       <c r="D10" s="8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>32</v>
       </c>
@@ -2332,7 +2356,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -2346,7 +2370,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
@@ -2360,7 +2384,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -2374,7 +2398,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>46</v>
       </c>
@@ -2387,8 +2411,11 @@
       <c r="D15" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>50</v>
       </c>
@@ -2402,7 +2429,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>52</v>
       </c>
@@ -2416,7 +2443,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>54</v>
       </c>
@@ -2430,7 +2457,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>58</v>
       </c>
@@ -2444,7 +2471,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>60</v>
       </c>
@@ -2458,7 +2485,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>62</v>
       </c>
@@ -2472,7 +2499,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>65</v>
       </c>
@@ -2486,7 +2513,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>68</v>
       </c>
@@ -2500,7 +2527,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>72</v>
       </c>
@@ -2514,7 +2541,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>75</v>
       </c>
@@ -2528,7 +2555,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>78</v>
       </c>
@@ -2542,7 +2569,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>80</v>
       </c>
@@ -2556,7 +2583,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>84</v>
       </c>
@@ -2570,7 +2597,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>86</v>
       </c>
@@ -2584,7 +2611,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>88</v>
       </c>
@@ -2598,7 +2625,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>91</v>
       </c>
@@ -2612,7 +2639,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>94</v>
       </c>
@@ -2626,7 +2653,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>97</v>
       </c>
@@ -2640,7 +2667,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>101</v>
       </c>
@@ -2654,7 +2681,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>104</v>
       </c>
@@ -2668,7 +2695,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>108</v>
       </c>
@@ -2682,7 +2709,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>111</v>
       </c>
@@ -2696,7 +2723,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>115</v>
       </c>
@@ -2710,7 +2737,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>118</v>
       </c>
@@ -2724,7 +2751,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>121</v>
       </c>
@@ -2738,7 +2765,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>124</v>
       </c>
@@ -2752,7 +2779,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>127</v>
       </c>
@@ -2766,7 +2793,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>130</v>
       </c>
@@ -2780,7 +2807,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>133</v>
       </c>
@@ -2794,7 +2821,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>136</v>
       </c>
@@ -2808,7 +2835,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>140</v>
       </c>
@@ -2822,7 +2849,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>144</v>
       </c>
@@ -2836,7 +2863,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>148</v>
       </c>
@@ -2850,7 +2877,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>150</v>
       </c>
@@ -2864,7 +2891,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>153</v>
       </c>
@@ -2878,7 +2905,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>156</v>
       </c>
@@ -2892,7 +2919,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>159</v>
       </c>
@@ -2906,7 +2933,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>163</v>
       </c>
@@ -2920,7 +2947,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>167</v>
       </c>
@@ -2934,7 +2961,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>169</v>
       </c>
@@ -2948,7 +2975,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>172</v>
       </c>
@@ -2962,7 +2989,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>175</v>
       </c>
@@ -2976,7 +3003,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>178</v>
       </c>
@@ -2990,7 +3017,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>181</v>
       </c>
@@ -3004,7 +3031,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>183</v>
       </c>
@@ -3018,7 +3045,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>186</v>
       </c>
@@ -3032,7 +3059,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>189</v>
       </c>
@@ -3046,7 +3073,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>191</v>
       </c>
@@ -3060,7 +3087,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>194</v>
       </c>
@@ -3074,7 +3101,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>198</v>
       </c>
@@ -3088,7 +3115,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>201</v>
       </c>
@@ -3102,7 +3129,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>204</v>
       </c>
@@ -3116,7 +3143,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>208</v>
       </c>
@@ -3130,7 +3157,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
         <v>210</v>
       </c>
@@ -3144,7 +3171,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>212</v>
       </c>
@@ -3158,7 +3185,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
         <v>215</v>
       </c>
@@ -3172,7 +3199,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>218</v>
       </c>
@@ -3186,7 +3213,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
         <v>220</v>
       </c>
@@ -3200,7 +3227,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>222</v>
       </c>
@@ -3214,7 +3241,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
         <v>224</v>
       </c>
@@ -3228,7 +3255,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>228</v>
       </c>
@@ -3242,7 +3269,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
         <v>231</v>
       </c>
@@ -3256,7 +3283,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>234</v>
       </c>
@@ -3270,7 +3297,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
         <v>238</v>
       </c>
@@ -3284,7 +3311,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>242</v>
       </c>
@@ -3298,7 +3325,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>246</v>
       </c>
@@ -3312,7 +3339,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>249</v>
       </c>
@@ -3326,7 +3353,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
         <v>252</v>
       </c>
@@ -3340,7 +3367,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>256</v>
       </c>
@@ -3354,7 +3381,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>259</v>
       </c>
@@ -3368,7 +3395,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
         <v>262</v>
       </c>
@@ -3382,7 +3409,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>265</v>
       </c>
@@ -3396,7 +3423,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>268</v>
       </c>
@@ -3410,7 +3437,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
         <v>270</v>
       </c>
@@ -3424,7 +3451,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>272</v>
       </c>
@@ -3438,7 +3465,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
         <v>275</v>
       </c>
@@ -3452,7 +3479,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
         <v>279</v>
       </c>
@@ -3466,7 +3493,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="s">
         <v>282</v>
       </c>
@@ -3480,7 +3507,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>286</v>
       </c>
@@ -3494,7 +3521,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
         <v>288</v>
       </c>
@@ -3508,7 +3535,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
         <v>291</v>
       </c>
@@ -3522,7 +3549,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="s">
         <v>295</v>
       </c>
@@ -3536,7 +3563,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
         <v>298</v>
       </c>
@@ -3550,7 +3577,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>300</v>
       </c>
@@ -3564,7 +3591,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>303</v>
       </c>
@@ -3578,7 +3605,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
         <v>305</v>
       </c>
@@ -3592,7 +3619,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>309</v>
       </c>
@@ -3606,7 +3633,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="4" t="s">
         <v>312</v>
       </c>
@@ -3620,7 +3647,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>315</v>
       </c>
@@ -3634,7 +3661,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="4" t="s">
         <v>318</v>
       </c>
@@ -3648,7 +3675,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
         <v>321</v>
       </c>
@@ -3662,7 +3689,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="4" t="s">
         <v>323</v>
       </c>
@@ -3676,7 +3703,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
         <v>325</v>
       </c>
@@ -3690,7 +3717,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="s">
         <v>328</v>
       </c>
@@ -3704,7 +3731,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>332</v>
       </c>
@@ -3718,7 +3745,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
         <v>335</v>
       </c>
@@ -3732,7 +3759,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
         <v>338</v>
       </c>
@@ -3746,7 +3773,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="4" t="s">
         <v>341</v>
       </c>
@@ -3760,7 +3787,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
         <v>344</v>
       </c>
@@ -3774,7 +3801,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="4" t="s">
         <v>346</v>
       </c>
@@ -3788,7 +3815,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
         <v>350</v>
       </c>
@@ -3802,7 +3829,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="4" t="s">
         <v>353</v>
       </c>
@@ -3816,7 +3843,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
         <v>356</v>
       </c>
@@ -3830,7 +3857,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
         <v>359</v>
       </c>
@@ -3844,7 +3871,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
         <v>362</v>
       </c>
@@ -3858,7 +3885,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" ht="45.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
         <v>365</v>
       </c>
@@ -3872,7 +3899,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="s">
         <v>368</v>
       </c>
@@ -3886,7 +3913,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>371</v>
       </c>
@@ -3900,7 +3927,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
         <v>374</v>
       </c>
@@ -3914,7 +3941,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="s">
         <v>377</v>
       </c>
@@ -3928,7 +3955,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="s">
         <v>380</v>
       </c>
@@ -3942,7 +3969,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
         <v>383</v>
       </c>
@@ -3956,7 +3983,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="s">
         <v>386</v>
       </c>
@@ -3970,7 +3997,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
         <v>389</v>
       </c>
@@ -3984,7 +4011,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="s">
         <v>393</v>
       </c>
@@ -3998,7 +4025,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="4" t="s">
         <v>396</v>
       </c>
@@ -4012,7 +4039,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
         <v>398</v>
       </c>
@@ -4026,7 +4053,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="s">
         <v>400</v>
       </c>
@@ -4040,7 +4067,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
         <v>403</v>
       </c>
@@ -4054,7 +4081,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="s">
         <v>405</v>
       </c>
@@ -4068,7 +4095,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>407</v>
       </c>
@@ -4082,7 +4109,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
         <v>410</v>
       </c>
@@ -4096,7 +4123,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
         <v>414</v>
       </c>
@@ -4110,7 +4137,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="s">
         <v>418</v>
       </c>
@@ -4124,7 +4151,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="s">
         <v>421</v>
       </c>
@@ -4138,7 +4165,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="s">
         <v>425</v>
       </c>
@@ -4152,7 +4179,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
         <v>429</v>
       </c>
@@ -4166,7 +4193,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="4" t="s">
         <v>432</v>
       </c>
@@ -4180,7 +4207,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="3" t="s">
         <v>435</v>
       </c>
@@ -4194,7 +4221,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="4" t="s">
         <v>437</v>
       </c>
@@ -4208,7 +4235,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="3" t="s">
         <v>440</v>
       </c>
@@ -4222,7 +4249,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="4" t="s">
         <v>442</v>
       </c>
@@ -4236,7 +4263,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A148" s="3" t="s">
         <v>443</v>
       </c>
@@ -4250,7 +4277,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="4" t="s">
         <v>446</v>
       </c>
@@ -4264,7 +4291,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A150" s="3" t="s">
         <v>450</v>
       </c>
@@ -4278,7 +4305,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A151" s="4" t="s">
         <v>452</v>
       </c>
@@ -4292,7 +4319,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="3" t="s">
         <v>456</v>
       </c>
@@ -4306,7 +4333,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A153" s="4" t="s">
         <v>459</v>
       </c>
@@ -4320,7 +4347,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="3" t="s">
         <v>461</v>
       </c>
@@ -4334,7 +4361,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="4" t="s">
         <v>463</v>
       </c>
@@ -4348,7 +4375,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="3" t="s">
         <v>466</v>
       </c>
@@ -4362,7 +4389,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A157" s="4" t="s">
         <v>469</v>
       </c>
@@ -4376,7 +4403,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="3" t="s">
         <v>472</v>
       </c>
@@ -4390,7 +4417,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="4" t="s">
         <v>476</v>
       </c>
@@ -4404,7 +4431,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A160" s="3" t="s">
         <v>479</v>
       </c>
@@ -4418,7 +4445,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A161" s="4" t="s">
         <v>482</v>
       </c>
@@ -4432,7 +4459,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A162" s="3" t="s">
         <v>484</v>
       </c>
@@ -4446,7 +4473,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A163" s="4" t="s">
         <v>487</v>
       </c>
@@ -4460,7 +4487,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A164" s="3" t="s">
         <v>490</v>
       </c>
@@ -4474,7 +4501,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A165" s="4" t="s">
         <v>492</v>
       </c>
@@ -4488,7 +4515,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A166" s="3" t="s">
         <v>496</v>
       </c>
@@ -4502,7 +4529,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A167" s="4" t="s">
         <v>499</v>
       </c>
@@ -4516,7 +4543,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A168" s="3" t="s">
         <v>503</v>
       </c>
@@ -4530,7 +4557,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A169" s="4" t="s">
         <v>507</v>
       </c>
@@ -4544,7 +4571,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A170" s="3" t="s">
         <v>511</v>
       </c>
@@ -4558,7 +4585,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A171" s="4" t="s">
         <v>514</v>
       </c>
@@ -4572,7 +4599,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A172" s="3" t="s">
         <v>516</v>
       </c>
@@ -4586,7 +4613,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A173" s="4" t="s">
         <v>519</v>
       </c>
@@ -4600,7 +4627,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A174" s="3" t="s">
         <v>522</v>
       </c>
@@ -4614,7 +4641,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A175" s="4" t="s">
         <v>525</v>
       </c>
@@ -4628,7 +4655,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A176" s="3" t="s">
         <v>528</v>
       </c>
@@ -4642,7 +4669,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A177" s="4" t="s">
         <v>532</v>
       </c>
@@ -4656,7 +4683,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A178" s="3" t="s">
         <v>534</v>
       </c>
@@ -4670,7 +4697,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A179" s="4" t="s">
         <v>536</v>
       </c>
@@ -4684,7 +4711,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A180" s="3" t="s">
         <v>539</v>
       </c>
@@ -4698,7 +4725,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A181" s="4" t="s">
         <v>543</v>
       </c>
@@ -4712,7 +4739,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A182" s="3" t="s">
         <v>547</v>
       </c>
@@ -4726,7 +4753,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A183" s="4" t="s">
         <v>550</v>
       </c>
@@ -4740,7 +4767,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A184" s="3" t="s">
         <v>552</v>
       </c>
@@ -4754,7 +4781,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A185" s="4" t="s">
         <v>556</v>
       </c>
@@ -4768,7 +4795,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A186" s="3" t="s">
         <v>558</v>
       </c>
@@ -4782,7 +4809,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A187" s="4" t="s">
         <v>560</v>
       </c>
@@ -4796,7 +4823,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A188" s="3" t="s">
         <v>562</v>
       </c>
@@ -4810,7 +4837,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A189" s="4" t="s">
         <v>564</v>
       </c>
@@ -4824,7 +4851,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A190" s="3" t="s">
         <v>567</v>
       </c>
@@ -4838,7 +4865,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A191" s="4" t="s">
         <v>570</v>
       </c>
@@ -4860,14 +4887,172 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:Q25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>577</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>577</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>577</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4878,7 +5063,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>